<commit_message>
Update sample excel file for the excel-test-results-plugin
</commit_message>
<xml_diff>
--- a/excel-test-results-plugin/SampleExcelTestResults.xlsx
+++ b/excel-test-results-plugin/SampleExcelTestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\SpecSync\Samples\specsync-basic-calculator-specflow\MyCalculator.Specs\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693771F-72F0-4EB7-9879-6EF51AC5D1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED551FC-E437-452A-B53D-5E415D7ABC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4605" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Feature</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>NotExecuted</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>An OutOfRange error was thrown</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +407,7 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +420,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -429,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -443,7 +452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -457,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -471,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -483,6 +492,9 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>